<commit_message>
PCB BOM and CRC Check Added
</commit_message>
<xml_diff>
--- a/Schematic_Artifacts/Project Outputs for PSU4PSU/PSU4PSU.xlsx
+++ b/Schematic_Artifacts/Project Outputs for PSU4PSU/PSU4PSU.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AridDay\Desktop\PSU4PSU\Schematic_Artifacts\Project Outputs for PSU4PSU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5654E4C1-38CD-415B-A406-37932B7BB4E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1329AC55-97AD-4E87-BDB1-DA2130C08CEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{329F267F-12D1-4CDB-AC34-15097280C5CC}"/>
   </bookViews>
@@ -730,7 +730,7 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>